<commit_message>
- Actualización de templates
</commit_message>
<xml_diff>
--- a/Template/Export/Denominadores_D1_119.xlsx
+++ b/Template/Export/Denominadores_D1_119.xlsx
@@ -13,13 +13,11 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$AD$1</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -38,82 +36,82 @@
     <t>EpiYear</t>
   </si>
   <si>
-    <t>Grupo_edad</t>
-  </si>
-  <si>
-    <t>ETINumFem</t>
-  </si>
-  <si>
-    <t>ETINumMaso</t>
-  </si>
-  <si>
-    <t>ETINumST</t>
-  </si>
-  <si>
-    <t>ETINumEmerST</t>
-  </si>
-  <si>
-    <t>ETIDenoFem</t>
-  </si>
-  <si>
-    <t>ETIDenoMaso</t>
-  </si>
-  <si>
-    <t>ETIDenoST</t>
-  </si>
-  <si>
     <t>HospFem</t>
   </si>
   <si>
-    <t>HospMaso</t>
-  </si>
-  <si>
     <t>HospST</t>
   </si>
   <si>
-    <t>UCIFem</t>
-  </si>
-  <si>
-    <t>UCIMaso</t>
-  </si>
-  <si>
-    <t>UCIST</t>
-  </si>
-  <si>
-    <t>DefFem</t>
-  </si>
-  <si>
-    <t>DefMaso</t>
-  </si>
-  <si>
-    <t>DefST</t>
-  </si>
-  <si>
-    <t>NeuFem</t>
-  </si>
-  <si>
-    <t>NeuMaso</t>
-  </si>
-  <si>
-    <t>NeuST</t>
-  </si>
-  <si>
     <t>CCSARIFem</t>
   </si>
   <si>
-    <t>CCSARIMaso</t>
-  </si>
-  <si>
     <t>CCSARIST</t>
   </si>
   <si>
     <t>VentFem</t>
   </si>
   <si>
-    <t>VentMaso</t>
-  </si>
-  <si>
     <t>VentST</t>
+  </si>
+  <si>
+    <t>Age_Group</t>
+  </si>
+  <si>
+    <t>ILINumFem</t>
+  </si>
+  <si>
+    <t>ILINumMale</t>
+  </si>
+  <si>
+    <t>ILINumST</t>
+  </si>
+  <si>
+    <t>ILINumEmerST</t>
+  </si>
+  <si>
+    <t>ILIDenoFem</t>
+  </si>
+  <si>
+    <t>ILIDenoMale</t>
+  </si>
+  <si>
+    <t>ILIDenoST</t>
+  </si>
+  <si>
+    <t>HospMale</t>
+  </si>
+  <si>
+    <t>ICUFem</t>
+  </si>
+  <si>
+    <t>ICUMale</t>
+  </si>
+  <si>
+    <t>ICUST</t>
+  </si>
+  <si>
+    <t>DeathsFem</t>
+  </si>
+  <si>
+    <t>DeathsMale</t>
+  </si>
+  <si>
+    <t>DeathsST</t>
+  </si>
+  <si>
+    <t>PneuFem</t>
+  </si>
+  <si>
+    <t>PneuMale</t>
+  </si>
+  <si>
+    <t>PneuST</t>
+  </si>
+  <si>
+    <t>CCSARIMale</t>
+  </si>
+  <si>
+    <t>VentMale</t>
   </si>
 </sst>
 </file>
@@ -121,7 +119,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -169,8 +167,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,83 +526,83 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="N1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="P1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -612,28 +610,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>